<commit_message>
Updated model and work on UI.
</commit_message>
<xml_diff>
--- a/model/catalogue.xlsx
+++ b/model/catalogue.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="206">
   <si>
     <t>entity</t>
   </si>
@@ -155,9 +155,6 @@
     <t>label-xx</t>
   </si>
   <si>
-    <t>LifeCycle_Categories</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -182,12 +179,6 @@
     <t>position</t>
   </si>
   <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>LifeCycle_CoreVariables</t>
   </si>
   <si>
@@ -197,15 +188,9 @@
     <t>variable</t>
   </si>
   <si>
-    <t>Variable</t>
-  </si>
-  <si>
     <t>Short name of the variable (should not include spaces)</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Longer human readable name of the variable</t>
   </si>
   <si>
@@ -248,12 +233,6 @@
     <t>xref</t>
   </si>
   <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -263,9 +242,6 @@
     <t>parent</t>
   </si>
   <si>
-    <t>children</t>
-  </si>
-  <si>
     <t>one_to_many</t>
   </si>
   <si>
@@ -281,9 +257,6 @@
     <t>target</t>
   </si>
   <si>
-    <t>Position of the group in the list</t>
-  </si>
-  <si>
     <t>cohort</t>
   </si>
   <si>
@@ -596,18 +569,6 @@
     <t xml:space="preserve">Menu </t>
   </si>
   <si>
-    <t>LifeCycle_Menu</t>
-  </si>
-  <si>
-    <t>parent menu</t>
-  </si>
-  <si>
-    <t>child menu</t>
-  </si>
-  <si>
-    <t>variables</t>
-  </si>
-  <si>
     <t>pregnancy</t>
   </si>
   <si>
@@ -686,19 +647,13 @@
     <t>Child</t>
   </si>
   <si>
-    <t>section</t>
-  </si>
-  <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>LifeCycle_Sections</t>
-  </si>
-  <si>
     <t>html</t>
   </si>
   <si>
-    <t>Position in a group of related variables</t>
+    <t>Variable name</t>
+  </si>
+  <si>
+    <t>UI</t>
   </si>
 </sst>
 </file>
@@ -754,8 +709,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -797,7 +762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="47">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -816,6 +781,11 @@
     <cellStyle name="Gevolgde hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -834,6 +804,11 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1109,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X48"/>
+  <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1197,201 +1172,203 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>204</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1403,47 +1380,45 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -1455,47 +1430,47 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -1507,45 +1482,45 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1557,47 +1532,45 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>216</v>
+        <v>65</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>217</v>
+        <v>66</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>218</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -1609,155 +1582,153 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
+      <c r="W10" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <v>200</v>
-      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="1" t="s">
-        <v>220</v>
-      </c>
+      <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -1769,99 +1740,97 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
-      <c r="W13" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="W13" s="1"/>
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -1873,45 +1842,45 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -1923,74 +1892,72 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
-      <c r="V16" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>43</v>
@@ -2000,22 +1967,22 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -2027,50 +1994,50 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
+      <c r="S18" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
@@ -2079,50 +2046,50 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
+      <c r="S19" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
@@ -2131,45 +2098,47 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="F20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -2181,45 +2150,45 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>90</v>
+        <v>204</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -2231,47 +2200,47 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -2283,45 +2252,45 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -2333,50 +2302,50 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="F24" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R24" s="1"/>
-      <c r="S24" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
@@ -2385,50 +2354,48 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R25" s="1"/>
-      <c r="S25" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
@@ -2437,47 +2404,45 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -2489,45 +2454,45 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -2539,20 +2504,20 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>43</v>
@@ -2562,22 +2527,22 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -2589,50 +2554,50 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
+      <c r="S29" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
@@ -2641,47 +2606,45 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>66</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
@@ -2693,45 +2656,45 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
@@ -2743,45 +2706,45 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -2793,45 +2756,45 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
@@ -2843,752 +2806,40 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="1"/>
+        <v>203</v>
+      </c>
       <c r="F34" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+        <v>42</v>
+      </c>
       <c r="L34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="T35" s="1"/>
-      <c r="U35" s="1"/>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
-      <c r="U36" s="1"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-      <c r="X36" s="1"/>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
-      <c r="X40" s="1"/>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
-      <c r="W41" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="X41" s="1"/>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1"/>
-      <c r="V42" s="1"/>
-      <c r="W42" s="1"/>
-      <c r="X42" s="1"/>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
-      <c r="T44" s="1"/>
-      <c r="U44" s="1"/>
-      <c r="V44" s="1"/>
-      <c r="W44" s="1"/>
-      <c r="X44" s="1"/>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R45" s="1"/>
-      <c r="S45" s="1"/>
-      <c r="T45" s="1"/>
-      <c r="U45" s="1"/>
-      <c r="V45" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="W45" s="1"/>
-      <c r="X45" s="1"/>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P46" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-      <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
-      <c r="W46" s="1"/>
-      <c r="X46" s="1"/>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
-      <c r="W47" s="1"/>
-      <c r="X47" s="1"/>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3609,7 +2860,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3617,34 +2868,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3657,7 +2908,7 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A12" sqref="A12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3671,16 +2922,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
         <v>20</v>
@@ -3742,198 +2993,198 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="H4" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="H5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="H6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
         <v>105</v>
       </c>
-      <c r="C8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" t="s">
-        <v>114</v>
-      </c>
       <c r="H8" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="H9" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="H10" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="H11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>205</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="H12" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3946,7 +3197,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3961,7 +3214,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
         <v>20</v>
@@ -3969,13 +3222,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3993,22 +3246,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4028,7 +3281,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4039,138 +3292,138 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4190,7 +3443,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4198,42 +3451,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -4251,7 +3504,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4259,26 +3512,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -4302,134 +3555,134 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4452,21 +3705,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -4474,10 +3727,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -4485,10 +3738,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -4496,10 +3749,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="C5">
         <v>3</v>

</xml_diff>

<commit_message>
- Changed model to define the menu structure outside of the core variables. - Rewritten user interface to load menu from MOLGENIS entity (WIP). - Split up code.
</commit_message>
<xml_diff>
--- a/model/catalogue.xlsx
+++ b/model/catalogue.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="13" r:id="rId1"/>
@@ -19,9 +19,11 @@
     <sheet name="LifeCycle_Cohorts" sheetId="8" r:id="rId5"/>
     <sheet name="LifeCycle_Units" sheetId="9" r:id="rId6"/>
     <sheet name="LifeCycle_DataTypes" sheetId="10" r:id="rId7"/>
-    <sheet name="LifeCycle_Categories" sheetId="11" r:id="rId8"/>
-    <sheet name="LifeCycle_Sections" sheetId="14" r:id="rId9"/>
-    <sheet name="LifeCycle_Status" sheetId="12" r:id="rId10"/>
+    <sheet name="LifeCycle_Tags" sheetId="11" r:id="rId8"/>
+    <sheet name="LifeCycle_Status" sheetId="12" r:id="rId9"/>
+    <sheet name="LifeCycle_CoreVariables" sheetId="15" r:id="rId10"/>
+    <sheet name="LifeCycle_SourceVariables" sheetId="16" r:id="rId11"/>
+    <sheet name="LifeCycle_Harmonizations" sheetId="17" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="270">
   <si>
     <t>entity</t>
   </si>
@@ -407,33 +409,9 @@
     <t>continuous</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>binary</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>DNBC</t>
   </si>
   <si>
@@ -494,12 +472,6 @@
     <t>cm</t>
   </si>
   <si>
-    <t>days</t>
-  </si>
-  <si>
-    <t>years</t>
-  </si>
-  <si>
     <t>Binary</t>
   </si>
   <si>
@@ -524,9 +496,6 @@
     <t>Pre-school age (2-5 yrs)</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>School age (6-12 yrs)</t>
   </si>
   <si>
@@ -536,15 +505,9 @@
     <t>Young adulthood (18-29 yrs)</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>Adulthood (30+ yrs)</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>General information</t>
   </si>
   <si>
@@ -563,12 +526,6 @@
     <t>Missing</t>
   </si>
   <si>
-    <t>Menu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Menu </t>
-  </si>
-  <si>
     <t>pregnancy</t>
   </si>
   <si>
@@ -617,12 +574,6 @@
     <t>Categories of the core variables</t>
   </si>
   <si>
-    <t>Sections</t>
-  </si>
-  <si>
-    <t>Sections of the core variables</t>
-  </si>
-  <si>
     <t>meta</t>
   </si>
   <si>
@@ -653,7 +604,292 @@
     <t>Variable name</t>
   </si>
   <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>LifeCycle_Tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any maternal smoking during 3. trimester of pregnancy  </t>
+  </si>
+  <si>
+    <t>0 = no
+1 = yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maternal smoking during 3. trimester of pregnancy </t>
+  </si>
+  <si>
+    <t>PREG_SMK3</t>
+  </si>
+  <si>
+    <t>aaaacyc66k5rb6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any maternal smoking during 2. trimester of pregnancy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maternal smoking during 2. trimester of pregnancy </t>
+  </si>
+  <si>
+    <t>PREG_SMK2</t>
+  </si>
+  <si>
+    <t>aaaacyc66i5x76qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any maternal smoking during 1. trimester of pregnancy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maternal smoking during 1. trimester of pregnancy </t>
+  </si>
+  <si>
+    <t>PREG_SMK1</t>
+  </si>
+  <si>
+    <t>aaaacyc66gi2v6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any maternal smoking during pregnancy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maternal smoking during pregnancy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREG_SMK </t>
+  </si>
+  <si>
+    <t>aaaacyc66bb3t6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maternal smoking before pregnancy at any time prepartum. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maternal pre-pregnancy smoking </t>
+  </si>
+  <si>
+    <t>PREPREG_SMK</t>
+  </si>
+  <si>
+    <t>aaaacyc6556u76qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>aaaacyc67m5p56qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>Education of the mother measured between 1 year prepartum and 1 year postpartum. 
+Level of education based on the highest of on-going and completed education.  
+If more than one are declared (different time points, but within the defined time frame), using the highest level declared.</t>
+  </si>
+  <si>
+    <t>1 = High
+2 = Medium
+3 = Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maternal education </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT_EDU </t>
+  </si>
+  <si>
+    <t>aaaacyc66nrzd6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>Average number of cigarettes per a day before pregnancy. Any smoking prepartum</t>
+  </si>
+  <si>
+    <t>0 = None
+1 = &lt; 10 per day
+2 = ≥ 10 per day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-pregnancy smoking (quantity) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREPREG_CIG </t>
+  </si>
+  <si>
+    <t>aaaacyc66qian6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average number of cigarettes smoked per day during pregnancy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maternal smoking during pregnancy (quantity) </t>
+  </si>
+  <si>
+    <t>PREG_SMKCIG</t>
+  </si>
+  <si>
+    <t>aaaacyc66d7vh6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>Best clinical judgement of estimating gestational age based on cohort's own discretion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestational age (Best estimate) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GA_BEST </t>
+  </si>
+  <si>
+    <t>aaaacyc652izf6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestational age based on maternal report </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestational age (Maternal report) </t>
+  </si>
+  <si>
+    <t>GA_MR</t>
+  </si>
+  <si>
+    <t>aaaacyc65xhen6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestational age based on ultrasound </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestational age (Ultrasound) </t>
+  </si>
+  <si>
+    <t>GA_US</t>
+  </si>
+  <si>
+    <t>aaaacyc65u6bv6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestational age based on last menstrual period in days </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestational age (Last menstrual period) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GA_LMP </t>
+  </si>
+  <si>
+    <t>aaaacyc65setb6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>aaaacyc67ibsp6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highest educational level completed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone interview 1 (12 weeks) </t>
+  </si>
+  <si>
+    <t>1: Long further education or managers of larger companies.     
+2: Medium further education or managers of smaller companies                         
+3: Vocational training, skilled work (Upper secondary)
+4: Unskilled work                
+5: On-going education (attained from A157 - eliminate here, because it is wanted to have highest of on-going and completed)
+6: out of the labour market 
+7: unquantifiable</t>
+  </si>
+  <si>
+    <t>SOCSTA</t>
+  </si>
+  <si>
+    <t>aaaacyc67fxof6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicative of on-going education </t>
+  </si>
+  <si>
+    <t>What education are you attending?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone Interview 1 (12 weeks) </t>
+  </si>
+  <si>
+    <t>1. basic school , to 9th grade
+2. HTX (higher technical exam) or HHX (higher commercial exam)
+3. high school
+4. semi-skilled worker training
+5. basic commercial vocational training
+6. professional training
+7. other vocational training
+8. short further education, less than 3 years
+9. medium further education, more than 3-4 years
+10.long further higher education more than 4 years
+11.other education describe________________
+12.do not know
+13.do not want to answer</t>
+  </si>
+  <si>
+    <t>A158</t>
+  </si>
+  <si>
+    <t>aaaacyc67dgh76qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>Are you attending school or vocational training?</t>
+  </si>
+  <si>
+    <t>1. Yes
+2. No-&gt;A159
+3. Do not know-&gt;A159
+4. Do not want to answer-&gt;A159</t>
+  </si>
+  <si>
+    <t>A157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On-going education: 
+If A157 is coded as Yes,  then A158 was answered. 
+A158 will be recoded into three levels corresponding the explanation in the harmonised variable.
+1 (High education): 8+9+10
+2 (Medium education): 2+3+4+5+6+7
+3 (Low education): 1 
+99 (missing): 12+13
+Completed education: 
+The variables of 6 categories  will be recoded into three: 
+1 (High education): 1+2 
+2 (Medium education): 3
+3 (Low education): 4+6
+99 (Missing): 7
+Final variable for harmonisation: 
+Highest of on-going and completed educational level. </t>
+  </si>
+  <si>
+    <t>aaaacyc67dgh76qwh3nxvnaaae,aaaacyc67fxof6qwh3nxvnaaae,aaaacyc67ibsp6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>parent menu</t>
+  </si>
+  <si>
+    <t>variables</t>
+  </si>
+  <si>
     <t>UI</t>
+  </si>
+  <si>
+    <t>User Interface</t>
+  </si>
+  <si>
+    <t>UI_Menu</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Position of the menu item</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>title</t>
   </si>
 </sst>
 </file>
@@ -709,7 +945,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -757,12 +993,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="51">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -786,6 +1029,8 @@
     <cellStyle name="Gevolgde hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -809,6 +1054,8 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1084,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X34"/>
+  <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1230,7 +1477,7 @@
         <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>41</v>
@@ -1585,16 +1832,16 @@
         <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>188</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>71</v>
+        <v>191</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>44</v>
@@ -1629,29 +1876,27 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
-      <c r="W10" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>42</v>
@@ -1683,7 +1928,9 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
+      <c r="W11" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -1691,16 +1938,16 @@
         <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>42</v>
@@ -1743,16 +1990,16 @@
         <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>42</v>
@@ -1795,15 +2042,17 @@
         <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F14" s="1" t="s">
         <v>42</v>
       </c>
@@ -1845,17 +2094,17 @@
         <v>71</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>42</v>
@@ -1895,17 +2144,15 @@
         <v>71</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
         <v>44</v>
       </c>
@@ -1947,20 +2194,22 @@
         <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F17" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1973,16 +2222,16 @@
         <v>42</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>42</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -1997,10 +2246,10 @@
         <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>41</v>
@@ -2010,20 +2259,20 @@
         <v>42</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>42</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>42</v>
@@ -2032,12 +2281,10 @@
         <v>42</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R18" s="1"/>
-      <c r="S18" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
@@ -2049,10 +2296,10 @@
         <v>71</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>41</v>
@@ -2072,7 +2319,7 @@
         <v>44</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>42</v>
@@ -2088,7 +2335,7 @@
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -2098,20 +2345,18 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
         <v>42</v>
       </c>
@@ -2123,10 +2368,10 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>42</v>
@@ -2135,13 +2380,15 @@
         <v>42</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>42</v>
       </c>
       <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
+      <c r="S20" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
@@ -2153,15 +2400,17 @@
         <v>78</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>204</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>42</v>
       </c>
@@ -2173,10 +2422,10 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>42</v>
@@ -2203,17 +2452,15 @@
         <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>187</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
         <v>42</v>
       </c>
@@ -2225,10 +2472,10 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>42</v>
@@ -2255,17 +2502,19 @@
         <v>78</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>42</v>
@@ -2305,17 +2554,15 @@
         <v>78</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
         <v>44</v>
       </c>
@@ -2357,17 +2604,19 @@
         <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="F25" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>42</v>
@@ -2389,7 +2638,7 @@
         <v>42</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>42</v>
@@ -2407,13 +2656,13 @@
         <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
@@ -2439,7 +2688,7 @@
         <v>42</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>42</v>
@@ -2457,17 +2706,17 @@
         <v>78</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>42</v>
@@ -2507,20 +2756,20 @@
         <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -2533,16 +2782,16 @@
         <v>42</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>42</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -2557,10 +2806,10 @@
         <v>78</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>41</v>
@@ -2570,20 +2819,20 @@
         <v>42</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>42</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>42</v>
@@ -2592,12 +2841,10 @@
         <v>42</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R29" s="1"/>
-      <c r="S29" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
@@ -2606,13 +2853,13 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>41</v>
@@ -2622,20 +2869,20 @@
         <v>42</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>42</v>
@@ -2644,10 +2891,12 @@
         <v>42</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
+      <c r="S30" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
@@ -2659,10 +2908,10 @@
         <v>90</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>41</v>
@@ -2672,29 +2921,29 @@
         <v>42</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>42</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
@@ -2706,13 +2955,13 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>41</v>
@@ -2722,29 +2971,29 @@
         <v>42</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O32" s="1" t="s">
         <v>42</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -2759,10 +3008,10 @@
         <v>75</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>41</v>
@@ -2772,29 +3021,29 @@
         <v>42</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
@@ -2809,37 +3058,286 @@
         <v>75</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>42</v>
+      <c r="D35" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>265</v>
+      </c>
+      <c r="B36" t="s">
+        <v>268</v>
+      </c>
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" t="s">
+        <v>43</v>
+      </c>
+      <c r="L36" t="s">
+        <v>42</v>
+      </c>
+      <c r="M36" t="s">
+        <v>42</v>
+      </c>
+      <c r="N36" t="s">
+        <v>44</v>
+      </c>
+      <c r="O36" t="s">
+        <v>42</v>
+      </c>
+      <c r="P36" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>265</v>
+      </c>
+      <c r="B37" t="s">
+        <v>269</v>
+      </c>
+      <c r="C37" t="s">
+        <v>269</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>42</v>
+      </c>
+      <c r="G37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L37" t="s">
+        <v>44</v>
+      </c>
+      <c r="M37" t="s">
+        <v>44</v>
+      </c>
+      <c r="N37" t="s">
+        <v>42</v>
+      </c>
+      <c r="O37" t="s">
+        <v>42</v>
+      </c>
+      <c r="P37" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>265</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D38" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" t="s">
+        <v>265</v>
+      </c>
+      <c r="F38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" t="s">
+        <v>42</v>
+      </c>
+      <c r="L38" t="s">
+        <v>42</v>
+      </c>
+      <c r="M38" t="s">
+        <v>42</v>
+      </c>
+      <c r="N38" t="s">
+        <v>42</v>
+      </c>
+      <c r="O38" t="s">
+        <v>42</v>
+      </c>
+      <c r="P38" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>265</v>
+      </c>
+      <c r="B39" t="s">
+        <v>262</v>
+      </c>
+      <c r="C39" t="s">
+        <v>262</v>
+      </c>
+      <c r="D39" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" t="s">
+        <v>42</v>
+      </c>
+      <c r="L39" t="s">
+        <v>42</v>
+      </c>
+      <c r="M39" t="s">
+        <v>42</v>
+      </c>
+      <c r="N39" t="s">
+        <v>42</v>
+      </c>
+      <c r="O39" t="s">
+        <v>42</v>
+      </c>
+      <c r="P39" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>265</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" t="s">
+        <v>266</v>
+      </c>
+      <c r="F40" t="s">
+        <v>42</v>
+      </c>
+      <c r="G40" t="s">
+        <v>42</v>
+      </c>
+      <c r="L40" t="s">
+        <v>42</v>
+      </c>
+      <c r="M40" t="s">
+        <v>42</v>
+      </c>
+      <c r="N40" t="s">
+        <v>42</v>
+      </c>
+      <c r="O40" t="s">
+        <v>42</v>
+      </c>
+      <c r="P40" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>42</v>
+      </c>
+      <c r="V40" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2850,52 +3348,480 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>39</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>243</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+      <c r="C2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" t="s">
         <v>189</v>
       </c>
+      <c r="G3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>220</v>
+      </c>
+      <c r="G6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>220</v>
+      </c>
+      <c r="G7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>215</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" t="s">
+        <v>193</v>
+      </c>
+      <c r="G9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" t="s">
+        <v>193</v>
+      </c>
+      <c r="G11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" t="s">
+        <v>193</v>
+      </c>
+      <c r="G13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" t="s">
+        <v>256</v>
+      </c>
+      <c r="I2" t="s">
+        <v>255</v>
+      </c>
+      <c r="J2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
       <c r="B3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H3" t="s">
+        <v>250</v>
+      </c>
+      <c r="I3" t="s">
+        <v>249</v>
+      </c>
+      <c r="J3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G4" t="s">
+        <v>245</v>
+      </c>
+      <c r="I4" t="s">
+        <v>244</v>
+      </c>
+      <c r="J4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B5" t="s">
-        <v>174</v>
+      <c r="G2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I2" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2905,16 +3831,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:H12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
@@ -3010,11 +3937,14 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
         <v>96</v>
       </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
       <c r="D3" t="s">
         <v>42</v>
       </c>
@@ -3022,12 +3952,12 @@
         <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
         <v>96</v>
@@ -3036,15 +3966,15 @@
         <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>193</v>
+        <v>102</v>
       </c>
       <c r="H4" t="s">
-        <v>194</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
         <v>96</v>
@@ -3053,15 +3983,15 @@
         <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="H5" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
         <v>96</v>
@@ -3070,69 +4000,72 @@
         <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
         <v>96</v>
       </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
       <c r="D7" t="s">
         <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
         <v>96</v>
       </c>
-      <c r="C8" t="s">
-        <v>90</v>
-      </c>
       <c r="D8" t="s">
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
         <v>96</v>
       </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
       <c r="D9" t="s">
         <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="H9" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
         <v>96</v>
@@ -3144,47 +4077,10 @@
         <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H11" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>175</v>
-      </c>
-      <c r="B12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>175</v>
-      </c>
-      <c r="H12" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3195,10 +4091,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3229,6 +4125,14 @@
       </c>
       <c r="C2" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3292,138 +4196,138 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3436,7 +4340,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3451,18 +4355,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3475,18 +4379,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3512,10 +4416,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3523,7 +4427,7 @@
         <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3531,7 +4435,7 @@
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3541,10 +4445,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3553,136 +4457,132 @@
     <col min="2" max="2" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" t="s">
         <v>157</v>
       </c>
-      <c r="C2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>178</v>
       </c>
-      <c r="B3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>179</v>
       </c>
-      <c r="B4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>180</v>
       </c>
-      <c r="B5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>181</v>
       </c>
-      <c r="B6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>182</v>
-      </c>
-      <c r="B7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>183</v>
-      </c>
-      <c r="B8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B9" t="s">
-        <v>165</v>
-      </c>
-      <c r="C9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>184</v>
-      </c>
-      <c r="B10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B16" t="s">
         <v>185</v>
-      </c>
-      <c r="B11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>186</v>
-      </c>
-      <c r="B12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C12" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3692,70 +4592,52 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>201</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Model fixes - Add harmonization status and syntax button to popup (WIP)
</commit_message>
<xml_diff>
--- a/model/catalogue.xlsx
+++ b/model/catalogue.xlsx
@@ -17,14 +17,13 @@
     <sheet name="LifeCycle_DataTypes" r:id="rId11" sheetId="9"/>
     <sheet name="LifeCycle_SourceVariables" r:id="rId12" sheetId="10"/>
     <sheet name="LifeCycle_Status" r:id="rId13" sheetId="11"/>
-    <sheet name="LifeCycle_Tags" r:id="rId14" sheetId="12"/>
-    <sheet name="LifeCycle_Units" r:id="rId15" sheetId="13"/>
+    <sheet name="LifeCycle_Units" r:id="rId14" sheetId="12"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="261">
   <si>
     <t>entity</t>
   </si>
@@ -182,7 +181,7 @@
     <t>variable</t>
   </si>
   <si>
-    <t>Variable name</t>
+    <t>Variable</t>
   </si>
   <si>
     <t>Short name of the variable (should not include spaces)</t>
@@ -206,12 +205,15 @@
     <t>values</t>
   </si>
   <si>
-    <t>Acceptable values</t>
+    <t>Values</t>
   </si>
   <si>
     <t>text</t>
   </si>
   <si>
+    <t>Acceptable values for the variable.</t>
+  </si>
+  <si>
     <t>unit</t>
   </si>
   <si>
@@ -221,51 +223,54 @@
     <t>LifeCycle_Units</t>
   </si>
   <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>LifeCycle_Status</t>
+  </si>
+  <si>
     <t>comments</t>
   </si>
   <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Tags</t>
+    <t>harmonizations</t>
+  </si>
+  <si>
+    <t>Harmonized variables</t>
+  </si>
+  <si>
+    <t>one_to_many</t>
+  </si>
+  <si>
+    <t>LifeCycle_Harmonizations</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>cohort</t>
+  </si>
+  <si>
+    <t>Cohort</t>
+  </si>
+  <si>
+    <t>xref</t>
+  </si>
+  <si>
+    <t>sources</t>
+  </si>
+  <si>
+    <t>Source variables</t>
   </si>
   <si>
     <t>mref</t>
   </si>
   <si>
-    <t>LifeCycle_Tags</t>
-  </si>
-  <si>
-    <t>harmonizations</t>
-  </si>
-  <si>
-    <t>Harmonized variables</t>
-  </si>
-  <si>
-    <t>one_to_many</t>
-  </si>
-  <si>
-    <t>LifeCycle_Harmonizations</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>cohort</t>
-  </si>
-  <si>
-    <t>Cohort</t>
-  </si>
-  <si>
-    <t>xref</t>
-  </si>
-  <si>
-    <t>sources</t>
-  </si>
-  <si>
-    <t>Source variables</t>
-  </si>
-  <si>
     <t>LifeCycle_SourceVariables</t>
   </si>
   <si>
@@ -281,24 +286,42 @@
     <t>status</t>
   </si>
   <si>
-    <t>Status of harmonization</t>
-  </si>
-  <si>
-    <t>LifeCycle_Status</t>
-  </si>
-  <si>
     <t>targetLabel</t>
   </si>
   <si>
     <t>sourceLabel</t>
   </si>
   <si>
+    <t>dateOfUpdate</t>
+  </si>
+  <si>
+    <t>Date of update</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Date the harmonization was last updated.</t>
+  </si>
+  <si>
     <t>collectionType</t>
   </si>
   <si>
     <t>Collection type</t>
   </si>
   <si>
+    <t>Date that the variable was last updated for harmonization.</t>
+  </si>
+  <si>
+    <t>dependencies</t>
+  </si>
+  <si>
+    <t>Dependencies</t>
+  </si>
+  <si>
+    <t>Description of dependencies of the variable on other variables.</t>
+  </si>
+  <si>
     <t>cohortLabel</t>
   </si>
   <si>
@@ -398,12 +421,6 @@
     <t>Status of the harmonization</t>
   </si>
   <si>
-    <t>Categories</t>
-  </si>
-  <si>
-    <t>Categories of the core variables</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -452,31 +469,37 @@
     <t>10</t>
   </si>
   <si>
+    <t>aaaacyfwrc3v36qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>Meta Variables</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Maternal Characteristics</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>aaaacyf3e2b776qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>Lifestyle Characteristics</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>aaaacyfxiuikf6qwh3nxvnaaae</t>
   </si>
   <si>
-    <t>Lifestyle Characteristics</t>
+    <t>Smoking</t>
   </si>
   <si>
     <t>aaaacyc66bb3t6qwh3nxvnaaae,aaaacyc66gi2v6qwh3nxvnaaae,aaaacyc66i5x76qwh3nxvnaaae,aaaacyc66k5rb6qwh3nxvnaaae,aaaacyc66d7vh6qwh3nxvnaaae,aaaacyc66qian6qwh3nxvnaaae,aaaacyc6556u76qwh3nxvnaaae</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>aaaacyfwrc3v36qwh3nxvnaaae</t>
-  </si>
-  <si>
-    <t>Meta Variables</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Maternal Characteristics</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>DNBC</t>
@@ -529,37 +552,37 @@
     <t>GECKO</t>
   </si>
   <si>
+    <t>HBCS</t>
+  </si>
+  <si>
+    <t>INMA</t>
+  </si>
+  <si>
+    <t>MoBa</t>
+  </si>
+  <si>
+    <t>NFBC66</t>
+  </si>
+  <si>
+    <t>NFBC86</t>
+  </si>
+  <si>
+    <t>NINFEA</t>
+  </si>
+  <si>
+    <t>RAINE</t>
+  </si>
+  <si>
+    <t>RHEA</t>
+  </si>
+  <si>
+    <t>SWS</t>
+  </si>
+  <si>
     <t>GenR</t>
   </si>
   <si>
-    <t>Generation R</t>
-  </si>
-  <si>
-    <t>HBCS</t>
-  </si>
-  <si>
-    <t>INMA</t>
-  </si>
-  <si>
-    <t>MoBa</t>
-  </si>
-  <si>
-    <t>NFBC66</t>
-  </si>
-  <si>
-    <t>NFBC86</t>
-  </si>
-  <si>
-    <t>NINFEA</t>
-  </si>
-  <si>
-    <t>RAINE</t>
-  </si>
-  <si>
-    <t>RHEA</t>
-  </si>
-  <si>
-    <t>SWS</t>
+    <t>Gen R</t>
   </si>
   <si>
     <t>aaaacyc65setb6qwh3nxvnaaae</t>
@@ -645,6 +668,73 @@
     <t>Average number of cigarettes per a day before pregnancy. Any smoking prepartum</t>
   </si>
   <si>
+    <t>aaaacyc6556u76qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>PREPREG_SMK</t>
+  </si>
+  <si>
+    <t>Maternal pre-pregnancy smoking</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>0 = no
+1 = yes</t>
+  </si>
+  <si>
+    <t>Maternal smoking before pregnancy at any time prepartum.</t>
+  </si>
+  <si>
+    <t>aaaacyc66bb3t6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>PREG_SMK</t>
+  </si>
+  <si>
+    <t>Maternal smoking during pregnancy</t>
+  </si>
+  <si>
+    <t>Any maternal smoking during pregnancy.</t>
+  </si>
+  <si>
+    <t>aaaacyc66gi2v6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>PREG_SMK1</t>
+  </si>
+  <si>
+    <t>Maternal smoking during 1. trimester of pregnancy</t>
+  </si>
+  <si>
+    <t>Any maternal smoking during 1. trimester of pregnancy</t>
+  </si>
+  <si>
+    <t>aaaacyc66i5x76qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>PREG_SMK2</t>
+  </si>
+  <si>
+    <t>Maternal smoking during 2. trimester of pregnancy</t>
+  </si>
+  <si>
+    <t>Any maternal smoking during 2. trimester of pregnancy</t>
+  </si>
+  <si>
+    <t>aaaacyc66k5rb6qwh3nxvnaaae</t>
+  </si>
+  <si>
+    <t>PREG_SMK3</t>
+  </si>
+  <si>
+    <t>Maternal smoking during 3. trimester of pregnancy</t>
+  </si>
+  <si>
+    <t>Any maternal smoking during 3. trimester of pregnancy</t>
+  </si>
+  <si>
     <t>Maternal education</t>
   </si>
   <si>
@@ -653,76 +743,12 @@
 3 = Low</t>
   </si>
   <si>
+    <t>partial</t>
+  </si>
+  <si>
     <t>Education of the mother measured between 1 year prepartum and 1 year postpartum. 
 Level of education based on the highest of on-going and completed education.  
 If more than one are declared (different time points, but within the defined time frame), using the highest level declared.</t>
-  </si>
-  <si>
-    <t>aaaacyc6556u76qwh3nxvnaaae</t>
-  </si>
-  <si>
-    <t>PREPREG_SMK</t>
-  </si>
-  <si>
-    <t>Maternal pre-pregnancy smoking</t>
-  </si>
-  <si>
-    <t>binary</t>
-  </si>
-  <si>
-    <t>0 = no
-1 = yes</t>
-  </si>
-  <si>
-    <t>Maternal smoking before pregnancy at any time prepartum.</t>
-  </si>
-  <si>
-    <t>aaaacyc66bb3t6qwh3nxvnaaae</t>
-  </si>
-  <si>
-    <t>PREG_SMK</t>
-  </si>
-  <si>
-    <t>Maternal smoking during pregnancy</t>
-  </si>
-  <si>
-    <t>Any maternal smoking during pregnancy.</t>
-  </si>
-  <si>
-    <t>aaaacyc66gi2v6qwh3nxvnaaae</t>
-  </si>
-  <si>
-    <t>PREG_SMK1</t>
-  </si>
-  <si>
-    <t>Maternal smoking during 1. trimester of pregnancy</t>
-  </si>
-  <si>
-    <t>Any maternal smoking during 1. trimester of pregnancy</t>
-  </si>
-  <si>
-    <t>aaaacyc66i5x76qwh3nxvnaaae</t>
-  </si>
-  <si>
-    <t>PREG_SMK2</t>
-  </si>
-  <si>
-    <t>Maternal smoking during 2. trimester of pregnancy</t>
-  </si>
-  <si>
-    <t>Any maternal smoking during 2. trimester of pregnancy</t>
-  </si>
-  <si>
-    <t>aaaacyc66k5rb6qwh3nxvnaaae</t>
-  </si>
-  <si>
-    <t>PREG_SMK3</t>
-  </si>
-  <si>
-    <t>Maternal smoking during 3. trimester of pregnancy</t>
-  </si>
-  <si>
-    <t>Any maternal smoking during 3. trimester of pregnancy</t>
   </si>
   <si>
     <t>Binary</t>
@@ -773,9 +799,6 @@
     <t>What education are you attending?</t>
   </si>
   <si>
-    <t>Indicative of on-going education</t>
-  </si>
-  <si>
     <t>aaaacyc67fxof6qwh3nxvnaaae</t>
   </si>
   <si>
@@ -803,9 +826,6 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>partial</t>
-  </si>
-  <si>
     <t>Partial</t>
   </si>
   <si>
@@ -819,96 +839,6 @@
   </si>
   <si>
     <t>Missing</t>
-  </si>
-  <si>
-    <t>pregnancy</t>
-  </si>
-  <si>
-    <t>Pregnancy</t>
-  </si>
-  <si>
-    <t>delivery</t>
-  </si>
-  <si>
-    <t>Delivery</t>
-  </si>
-  <si>
-    <t>birth_outcome</t>
-  </si>
-  <si>
-    <t>Birth outcomes/neonatal period (0-1 month)</t>
-  </si>
-  <si>
-    <t>infancy</t>
-  </si>
-  <si>
-    <t>Infancy (1-23 months)</t>
-  </si>
-  <si>
-    <t>pre-school</t>
-  </si>
-  <si>
-    <t>Pre-school age (2-5 yrs)</t>
-  </si>
-  <si>
-    <t>school-age</t>
-  </si>
-  <si>
-    <t>School age (6-12 yrs)</t>
-  </si>
-  <si>
-    <t>adolesence</t>
-  </si>
-  <si>
-    <t>Adolescence (13-17 yrs)</t>
-  </si>
-  <si>
-    <t>young-adult</t>
-  </si>
-  <si>
-    <t>Young adulthood (18-29 yrs)</t>
-  </si>
-  <si>
-    <t>adult</t>
-  </si>
-  <si>
-    <t>Adulthood (30+ yrs)</t>
-  </si>
-  <si>
-    <t>general</t>
-  </si>
-  <si>
-    <t>General information</t>
-  </si>
-  <si>
-    <t>pre-pregnancy</t>
-  </si>
-  <si>
-    <t>Pre-pregnancy</t>
-  </si>
-  <si>
-    <t>meta</t>
-  </si>
-  <si>
-    <t>Meta variables</t>
-  </si>
-  <si>
-    <t>maternal</t>
-  </si>
-  <si>
-    <t>Maternal characteristics</t>
-  </si>
-  <si>
-    <t>paternal</t>
-  </si>
-  <si>
-    <t>Paternal characteristics</t>
-  </si>
-  <si>
-    <t>child</t>
-  </si>
-  <si>
-    <t>Child</t>
   </si>
   <si>
     <t>kg</t>
@@ -1402,22 +1332,25 @@
       <c r="Q9" t="s">
         <v>43</v>
       </c>
+      <c r="V9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
         <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
         <v>44</v>
@@ -1449,16 +1382,19 @@
         <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
         <v>43</v>
@@ -1487,10 +1423,10 @@
         <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
         <v>61</v>
@@ -1525,16 +1461,16 @@
         <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F13" t="s">
         <v>44</v>
@@ -1559,26 +1495,29 @@
       </c>
       <c r="Q13" t="s">
         <v>43</v>
+      </c>
+      <c r="W13" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s">
         <v>43</v>
@@ -1600,26 +1539,23 @@
       </c>
       <c r="Q14" t="s">
         <v>43</v>
-      </c>
-      <c r="W14" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
         <v>43</v>
@@ -1648,19 +1584,19 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
         <v>78</v>
       </c>
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
-      </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="F16" t="s">
         <v>43</v>
@@ -1689,19 +1625,16 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F17" t="s">
         <v>43</v>
@@ -1730,19 +1663,19 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="D18" t="s">
         <v>61</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
         <v>43</v>
@@ -1768,16 +1701,19 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
+        <v>68</v>
       </c>
       <c r="F19" t="s">
         <v>44</v>
@@ -1806,25 +1742,22 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G20" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="L20" t="s">
         <v>43</v>
@@ -1833,27 +1766,27 @@
         <v>43</v>
       </c>
       <c r="N20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O20" t="s">
         <v>43</v>
       </c>
       <c r="P20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
@@ -1862,7 +1795,7 @@
         <v>43</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L21" t="s">
         <v>43</v>
@@ -1871,7 +1804,7 @@
         <v>43</v>
       </c>
       <c r="N21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O21" t="s">
         <v>43</v>
@@ -1880,18 +1813,21 @@
         <v>43</v>
       </c>
       <c r="Q21" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="S21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
@@ -1903,10 +1839,10 @@
         <v>43</v>
       </c>
       <c r="L22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N22" t="s">
         <v>43</v>
@@ -1921,33 +1857,33 @@
         <v>43</v>
       </c>
       <c r="S22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G23" t="s">
         <v>43</v>
       </c>
       <c r="L23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N23" t="s">
         <v>43</v>
@@ -1956,27 +1892,27 @@
         <v>43</v>
       </c>
       <c r="P23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q23" t="s">
         <v>43</v>
       </c>
-      <c r="S23" t="s">
-        <v>75</v>
+      <c r="V23" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
         <v>39</v>
@@ -2000,7 +1936,7 @@
         <v>43</v>
       </c>
       <c r="P24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q24" t="s">
         <v>43</v>
@@ -2008,7 +1944,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
         <v>51</v>
@@ -2046,7 +1982,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
         <v>55</v>
@@ -2087,7 +2023,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
@@ -2125,19 +2061,19 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
         <v>57</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F28" t="s">
         <v>44</v>
@@ -2166,13 +2102,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D29" t="s">
         <v>42</v>
@@ -2204,7 +2140,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
         <v>21</v>
@@ -2242,16 +2178,16 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="F31" t="s">
         <v>44</v>
@@ -2276,26 +2212,29 @@
       </c>
       <c r="Q31" t="s">
         <v>43</v>
+      </c>
+      <c r="V31" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="F32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G32" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L32" t="s">
         <v>43</v>
@@ -2304,27 +2243,30 @@
         <v>43</v>
       </c>
       <c r="N32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O32" t="s">
         <v>43</v>
       </c>
       <c r="P32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q32" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="V32" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
@@ -2333,7 +2275,7 @@
         <v>43</v>
       </c>
       <c r="G33" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="L33" t="s">
         <v>43</v>
@@ -2342,7 +2284,7 @@
         <v>43</v>
       </c>
       <c r="N33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O33" t="s">
         <v>43</v>
@@ -2351,21 +2293,18 @@
         <v>43</v>
       </c>
       <c r="Q33" t="s">
-        <v>43</v>
-      </c>
-      <c r="S33" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
@@ -2374,7 +2313,7 @@
         <v>43</v>
       </c>
       <c r="G34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L34" t="s">
         <v>43</v>
@@ -2383,7 +2322,7 @@
         <v>43</v>
       </c>
       <c r="N34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O34" t="s">
         <v>43</v>
@@ -2392,18 +2331,21 @@
         <v>43</v>
       </c>
       <c r="Q34" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="S34" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>
@@ -2412,36 +2354,36 @@
         <v>43</v>
       </c>
       <c r="G35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O35" t="s">
         <v>43</v>
       </c>
       <c r="P35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D36" t="s">
         <v>42</v>
@@ -2450,36 +2392,36 @@
         <v>43</v>
       </c>
       <c r="G36" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L36" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M36" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O36" t="s">
         <v>43</v>
       </c>
       <c r="P36" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="D37" t="s">
         <v>42</v>
@@ -2488,54 +2430,51 @@
         <v>43</v>
       </c>
       <c r="G37" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="L37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O37" t="s">
         <v>43</v>
       </c>
       <c r="P37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="F38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G38" t="s">
         <v>43</v>
       </c>
       <c r="L38" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M38" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N38" t="s">
         <v>43</v>
@@ -2552,19 +2491,19 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E39" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="F39" t="s">
         <v>44</v>
@@ -2593,19 +2532,22 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D40" t="s">
-        <v>100</v>
+        <v>81</v>
+      </c>
+      <c r="E40" t="s">
+        <v>48</v>
       </c>
       <c r="F40" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G40" t="s">
         <v>43</v>
@@ -2623,13 +2565,51 @@
         <v>43</v>
       </c>
       <c r="P40" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q40" t="s">
         <v>43</v>
       </c>
-      <c r="V40" t="s">
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
         <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" t="s">
+        <v>43</v>
+      </c>
+      <c r="G41" t="s">
+        <v>43</v>
+      </c>
+      <c r="L41" t="s">
+        <v>43</v>
+      </c>
+      <c r="M41" t="s">
+        <v>43</v>
+      </c>
+      <c r="N41" t="s">
+        <v>43</v>
+      </c>
+      <c r="O41" t="s">
+        <v>43</v>
+      </c>
+      <c r="P41" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>43</v>
+      </c>
+      <c r="V41" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2647,7 +2627,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>51</v>
@@ -2659,103 +2639,103 @@
         <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G1" t="s">
         <v>21</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="I1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
-        <v>91</v>
+      <c r="K1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="F2" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="G2" t="s">
-        <v>232</v>
-      </c>
-      <c r="I2" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="J2" t="s">
-        <v>151</v>
+        <v>242</v>
+      </c>
+      <c r="K2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="C3" t="s">
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="F3" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="G3" t="s">
-        <v>236</v>
-      </c>
-      <c r="H3" t="s">
-        <v>237</v>
-      </c>
-      <c r="I3" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="J3" t="s">
-        <v>151</v>
+        <v>246</v>
+      </c>
+      <c r="K3" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="C4" t="s">
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="F4" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="G4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I4" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="J4" t="s">
-        <v>151</v>
+        <v>251</v>
+      </c>
+      <c r="K4" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2781,34 +2761,34 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="B3" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="B5" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2834,183 +2814,42 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>255</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>256</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>257</v>
+        <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>258</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B6" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>261</v>
-      </c>
-      <c r="B7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>263</v>
-      </c>
-      <c r="B8" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>267</v>
-      </c>
-      <c r="B10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>269</v>
-      </c>
-      <c r="B11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>271</v>
-      </c>
-      <c r="B12" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>273</v>
-      </c>
-      <c r="B13" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>275</v>
-      </c>
-      <c r="B14" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>277</v>
-      </c>
-      <c r="B15" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>279</v>
-      </c>
-      <c r="B16" t="s">
-        <v>280</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>281</v>
-      </c>
-      <c r="B2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>282</v>
-      </c>
-      <c r="B3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>283</v>
-      </c>
-      <c r="B6" t="s">
-        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3031,16 +2870,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
         <v>20</v>
@@ -3102,181 +2941,161 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="H2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
         <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="H3" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
         <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="H4" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="H5" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
         <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="H6" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D7" t="s">
         <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="H7" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D8" t="s">
         <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="H8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="H9" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="D10" t="s">
         <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3303,7 +3122,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E1" t="s">
         <v>20</v>
@@ -3311,24 +3130,24 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3346,22 +3165,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3379,75 +3198,89 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E4" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>154</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
       </c>
       <c r="E5" t="s">
-        <v>150</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3465,22 +3298,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>75</v>
-      </c>
-      <c r="B1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" t="s">
-        <v>74</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G1" t="s">
         <v>40</v>
@@ -3491,31 +3324,34 @@
       <c r="I1" t="s">
         <v>88</v>
       </c>
+      <c r="J1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="G2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="I2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3544,138 +3380,138 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B18" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3708,262 +3544,262 @@
         <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G2" t="s">
-        <v>179</v>
+        <v>186</v>
+      </c>
+      <c r="H2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F3" t="s">
-        <v>178</v>
-      </c>
-      <c r="G3" t="s">
-        <v>183</v>
+        <v>186</v>
+      </c>
+      <c r="H3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" t="s">
         <v>185</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>186</v>
       </c>
-      <c r="D4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F4" t="s">
-        <v>178</v>
-      </c>
-      <c r="G4" t="s">
-        <v>187</v>
+      <c r="H4" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D5" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F5" t="s">
-        <v>178</v>
-      </c>
-      <c r="G5" t="s">
-        <v>191</v>
+        <v>186</v>
+      </c>
+      <c r="H5" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C6" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>195</v>
-      </c>
-      <c r="G6" t="s">
-        <v>196</v>
+        <v>203</v>
+      </c>
+      <c r="H6" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
         <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>195</v>
-      </c>
-      <c r="G7" t="s">
-        <v>200</v>
+        <v>203</v>
+      </c>
+      <c r="H7" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>209</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>210</v>
       </c>
       <c r="C8" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>212</v>
       </c>
       <c r="E8" t="s">
-        <v>202</v>
-      </c>
-      <c r="G8" t="s">
-        <v>203</v>
-      </c>
-      <c r="J8" t="s">
-        <v>155</v>
+        <v>213</v>
+      </c>
+      <c r="H8" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="C9" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E9" t="s">
-        <v>208</v>
-      </c>
-      <c r="G9" t="s">
-        <v>209</v>
+        <v>213</v>
+      </c>
+      <c r="H9" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10" t="s">
         <v>212</v>
       </c>
-      <c r="D10" t="s">
-        <v>207</v>
-      </c>
       <c r="E10" t="s">
-        <v>208</v>
-      </c>
-      <c r="G10" t="s">
         <v>213</v>
+      </c>
+      <c r="H10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="C11" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="D11" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E11" t="s">
-        <v>208</v>
-      </c>
-      <c r="G11" t="s">
-        <v>217</v>
+        <v>213</v>
+      </c>
+      <c r="H11" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B12" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="C12" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D12" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E12" t="s">
-        <v>208</v>
-      </c>
-      <c r="G12" t="s">
-        <v>221</v>
+        <v>213</v>
+      </c>
+      <c r="H12" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>164</v>
       </c>
       <c r="C13" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="D13" t="s">
-        <v>207</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="G13" t="s">
-        <v>225</v>
+        <v>233</v>
+      </c>
+      <c r="H13" t="s">
+        <v>234</v>
+      </c>
+      <c r="I13" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3989,18 +3825,18 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4">
@@ -4008,7 +3844,7 @@
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>